<commit_message>
added greet45V snapshot and updated labels to electricity value
</commit_message>
<xml_diff>
--- a/merged_simulation_and_market_12min_2024-10-27.xlsx
+++ b/merged_simulation_and_market_12min_2024-10-27.xlsx
@@ -472,7 +472,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Combined_Energy_Difference_kWh</t>
+          <t>Combined_Electricity_Difference_kWh</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -487,7 +487,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Combined_Energy_Asset_Value_$</t>
+          <t>Combined_Electricity_Value_$</t>
         </is>
       </c>
     </row>

</xml_diff>